<commit_message>
update express tracking 2.0
</commit_message>
<xml_diff>
--- a/22_快递批量查询截图工具/Input/bill_number.xlsx
+++ b/22_快递批量查询截图工具/Input/bill_number.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9536DFF-50FD-4D48-BDDC-F588EDF53F2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AAF899-9AA2-48B0-814B-4A25973FAC28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>序号</t>
   </si>
@@ -36,14 +36,6 @@
   </si>
   <si>
     <t>369433311633</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2435435</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>34534543</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -429,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -455,51 +447,50 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -507,7 +498,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -515,14 +506,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -530,7 +521,7 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -559,20 +550,12 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A15"/>
+      <c r="B15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16"/>
+      <c r="B16"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17"/>
@@ -597,14 +580,6 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>